<commit_message>
Update Assignment 2 - Group 14.xlsx
</commit_message>
<xml_diff>
--- a/Assignment 2 - Group 14.xlsx
+++ b/Assignment 2 - Group 14.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AE0C54-AA82-4694-AE37-7FAB2D90341F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E564F1E-9205-44B8-AF9C-E0C9EF5961B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26565" yWindow="2700" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -232,12 +232,66 @@
   <si>
     <t>Cyber Security</t>
   </si>
+  <si>
+    <t>https://github.com/groupfourteen/assignment2.git</t>
+  </si>
+  <si>
+    <t>https://leevdb.github.io/Lee-van-den-Blink/</t>
+  </si>
+  <si>
+    <t>https://mdncb.github.io/assignment1/</t>
+  </si>
+  <si>
+    <t>https://atamosmusic.github.io/itprofile-assessment01.git.io/</t>
+  </si>
+  <si>
+    <t>repo link: https://github.com/Attikins/Attikins.github.io</t>
+  </si>
+  <si>
+    <t>https://njyoung95.github.io/NJYWebsite/</t>
+  </si>
+  <si>
+    <t>https://harryw77.github.io/Harrison_Assignment/</t>
+  </si>
+  <si>
+    <t>Individual Project Ideas</t>
+  </si>
+  <si>
+    <t>Smiling Game Saver</t>
+  </si>
+  <si>
+    <t>Game Programmer</t>
+  </si>
+  <si>
+    <t>Software Engineer - SDK (C++)</t>
+  </si>
+  <si>
+    <t>Moral Choice System Game - based around Batavia Mutiny of 1969</t>
+  </si>
+  <si>
+    <t>Nathan happy to work on layout for moment.  Something profesh.</t>
+  </si>
+  <si>
+    <t> Technical Lead @ Seventwenty </t>
+  </si>
+  <si>
+    <t>HUNTmap - Hardware Universal Networking Topological map</t>
+  </si>
+  <si>
+    <t>Level Designer/Scripter (Star Wars)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D role-playing game - modern design sensibilities, low fidelity graphics </t>
+  </si>
+  <si>
+    <t>1st draft completed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -284,8 +338,70 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0096CF"/>
+      <name val="Whitney"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212931"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +444,11 @@
         <bgColor rgb="FF6FA8DC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -353,10 +474,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -424,9 +548,26 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{BB83B773-1996-488D-811C-1C5547A92B6F}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -743,8 +884,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -769,11 +910,13 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
-        <v>2</v>
+      <c r="I1" s="2"/>
+      <c r="J1" s="35" t="s">
+        <v>73</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="K1" s="35" t="s">
+        <v>25</v>
+      </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -796,14 +939,22 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>67</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="J2" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>75</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -826,14 +977,22 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>68</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>76</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -850,20 +1009,28 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75">
+    <row r="4" spans="1:26" ht="15">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="J4" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" t="s">
+        <v>79</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -886,8 +1053,12 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>70</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -910,18 +1081,28 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" ht="12.75">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:26" ht="15">
+      <c r="A6" s="31" t="s">
+        <v>66</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>71</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -939,13 +1120,15 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="12.75">
-      <c r="A7" s="2"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
+      <c r="D7" s="32" t="s">
+        <v>16</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="34" t="s">
+        <v>72</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -968,40 +1151,20 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26" ht="56.25" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
+    <row r="8" spans="1:26" ht="12.75">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1018,23 +1181,39 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="12.75">
-      <c r="A9" s="7" t="s">
-        <v>19</v>
+    <row r="9" spans="1:26" ht="56.25" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
       </c>
-      <c r="B9" s="8">
-        <v>0.05</v>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10" t="s">
-        <v>20</v>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1052,24 +1231,24 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="25.5">
-      <c r="A10" s="11" t="s">
-        <v>21</v>
+    <row r="10" spans="1:26" ht="12.75">
+      <c r="A10" s="7" t="s">
+        <v>19</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13" t="s">
-        <v>22</v>
+      <c r="B10" s="8">
+        <v>0.05</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>23</v>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10" t="s">
+        <v>20</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1088,11 +1267,11 @@
     </row>
     <row r="11" spans="1:26" ht="25.5">
       <c r="A11" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>23</v>
@@ -1122,13 +1301,15 @@
     </row>
     <row r="12" spans="1:26" ht="25.5">
       <c r="A12" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -1152,18 +1333,22 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26" ht="12.75">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+    <row r="13" spans="1:26" ht="25.5">
+      <c r="A13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1181,21 +1366,17 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="12.75">
-      <c r="A14" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="22">
-        <v>0.05</v>
-      </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="10"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1212,22 +1393,22 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26" ht="25.5">
-      <c r="A15" s="11" t="s">
-        <v>28</v>
+    <row r="15" spans="1:26" ht="12.75">
+      <c r="A15" s="21" t="s">
+        <v>27</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13" t="s">
-        <v>29</v>
+      <c r="B15" s="22">
+        <v>0.05</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1244,21 +1425,25 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="51">
+    <row r="16" spans="1:26" ht="25.5">
       <c r="A16" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="F16" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
+      <c r="J16" s="37" t="s">
+        <v>78</v>
+      </c>
       <c r="K16" s="16"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1276,18 +1461,22 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26" ht="12.75">
-      <c r="A17" s="24"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+    <row r="17" spans="1:26" ht="51">
+      <c r="A17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="16"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1305,21 +1494,17 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26" ht="12.75">
-      <c r="A18" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="22">
-        <v>0.15</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="10"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1337,19 +1522,21 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" ht="12.75">
-      <c r="A19" s="11" t="s">
-        <v>33</v>
+      <c r="A19" s="21" t="s">
+        <v>32</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="16"/>
+      <c r="B19" s="22">
+        <v>0.15</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="10"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1367,8 +1554,8 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" ht="12.75">
-      <c r="A20" s="25" t="s">
-        <v>34</v>
+      <c r="A20" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -1397,17 +1584,19 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:26" ht="12.75">
-      <c r="A21" s="24"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="A21" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1425,21 +1614,17 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="12.75">
-      <c r="A22" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="22">
-        <v>0.15</v>
-      </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="10"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1456,24 +1641,22 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" spans="1:26" ht="25.5">
-      <c r="A23" s="25" t="s">
-        <v>36</v>
+    <row r="23" spans="1:26" ht="12.75">
+      <c r="A23" s="21" t="s">
+        <v>35</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="13" t="s">
-        <v>37</v>
+      <c r="B23" s="22">
+        <v>0.15</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="16"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="10"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1490,12 +1673,14 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" spans="1:26" ht="114.75">
-      <c r="A24" s="11" t="s">
-        <v>38</v>
+    <row r="24" spans="1:26" ht="25.5">
+      <c r="A24" s="25" t="s">
+        <v>36</v>
       </c>
       <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
+      <c r="C24" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15" t="s">
@@ -1522,18 +1707,22 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" spans="1:26" ht="12.75">
-      <c r="A25" s="24"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+    <row r="25" spans="1:26" ht="114.75">
+      <c r="A25" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1551,21 +1740,17 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="12.75">
-      <c r="A26" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="10"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1582,22 +1767,22 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" spans="1:26" ht="51">
-      <c r="A27" s="11" t="s">
-        <v>40</v>
+    <row r="27" spans="1:26" ht="12.75">
+      <c r="A27" s="21" t="s">
+        <v>39</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13" t="s">
-        <v>41</v>
+      <c r="B27" s="22">
+        <v>0.2</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="16"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="10"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1614,18 +1799,18 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28" spans="1:26" ht="12.75">
+    <row r="28" spans="1:26" ht="51">
       <c r="A28" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
+      <c r="C28" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
@@ -1646,22 +1831,24 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" spans="1:26" ht="12.75">
+    <row r="29" spans="1:26" ht="15">
       <c r="A29" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
       <c r="D29" s="15"/>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="16"/>
+      <c r="K29" s="42" t="s">
+        <v>83</v>
+      </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1680,16 +1867,16 @@
     </row>
     <row r="30" spans="1:26" ht="12.75">
       <c r="A30" s="11" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
       <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15" t="s">
+      <c r="E30" s="15" t="s">
         <v>23</v>
       </c>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
@@ -1712,14 +1899,16 @@
     </row>
     <row r="31" spans="1:26" ht="12.75">
       <c r="A31" s="11" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="G31" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -1741,17 +1930,19 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="1:26" ht="12.75">
-      <c r="A32" s="24"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="A32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="16"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -1769,21 +1960,17 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" spans="1:26" ht="12.75">
-      <c r="A33" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="22">
-        <v>0.1</v>
-      </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="10"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -1800,22 +1987,22 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34" spans="1:26" ht="38.25">
-      <c r="A34" s="11" t="s">
-        <v>45</v>
+    <row r="34" spans="1:26" ht="12.75">
+      <c r="A34" s="21" t="s">
+        <v>2</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="26" t="s">
-        <v>46</v>
+      <c r="B34" s="22">
+        <v>0.1</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="16"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="10"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -1832,13 +2019,13 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35" spans="1:26" ht="25.5">
+    <row r="35" spans="1:26" ht="38.25">
       <c r="A35" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35" s="12"/>
-      <c r="C35" s="11" t="s">
-        <v>48</v>
+      <c r="C35" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
@@ -1864,12 +2051,14 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36" spans="1:26" ht="12.75">
+    <row r="36" spans="1:26" ht="25.5">
       <c r="A36" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" s="12"/>
-      <c r="C36" s="13"/>
+      <c r="C36" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
@@ -1895,17 +2084,19 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" spans="1:26" ht="12.75">
-      <c r="A37" s="24"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="A37" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="16"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -1923,21 +2114,17 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38" spans="1:26" ht="12.75">
-      <c r="A38" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="10"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -1954,34 +2141,22 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" spans="1:26" ht="38.25">
-      <c r="A39" s="11" t="s">
-        <v>51</v>
+    <row r="39" spans="1:26" ht="12.75">
+      <c r="A39" s="21" t="s">
+        <v>50</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="13" t="s">
-        <v>52</v>
+      <c r="B39" s="27">
+        <v>0.1</v>
       </c>
-      <c r="D39" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J39" s="15"/>
-      <c r="K39" s="16"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="10"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -1998,18 +2173,34 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
     </row>
-    <row r="40" spans="1:26" ht="12.75">
-      <c r="A40" s="24"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+    <row r="40" spans="1:26" ht="38.25">
+      <c r="A40" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J40" s="15"/>
+      <c r="K40" s="16"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -2027,21 +2218,17 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" spans="1:26" ht="12.75">
-      <c r="A41" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="10"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -2059,19 +2246,21 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="12.75">
-      <c r="A42" s="11" t="s">
-        <v>54</v>
+      <c r="A42" s="21" t="s">
+        <v>53</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="16"/>
+      <c r="B42" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="C42" s="21"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="10"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -2090,12 +2279,10 @@
     </row>
     <row r="43" spans="1:26" ht="12.75">
       <c r="A43" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="C43" s="11"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
@@ -2121,17 +2308,21 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" spans="1:26" ht="12.75">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="2"/>
+      <c r="A44" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="16"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -2149,21 +2340,17 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="12.75">
-      <c r="A45" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="10"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -2181,17 +2368,21 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" ht="12.75">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
+      <c r="A46" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="10"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -29887,6 +30078,16 @@
       <c r="Z1034" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{EC11C092-6421-4E31-AC15-D7780FE8DAA5}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{735A258F-F30D-4428-B624-FB04919B028A}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{10148347-71C3-4476-AB40-51B878BB1E98}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{28C63A63-AC84-4A66-A669-91992A1B543E}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{1A433D49-B2D0-49F4-AABA-74603EFA264A}"/>
+    <hyperlink ref="E7" r:id="rId6" tooltip="https://harryw77.github.io/Harrison_Assignment/" xr:uid="{C4E733A4-72D1-42FF-86C6-B78730C9079D}"/>
+    <hyperlink ref="K6" r:id="rId7" display="https://ea.gr8people.com/index.gp?method=cappportal.showJob&amp;layoutid=2092&amp;inp1541=&amp;opportunityid=150448" xr:uid="{ABA94F6C-2733-45FC-A5C2-F989DA3AC21A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed html reports to docx
</commit_message>
<xml_diff>
--- a/Assignment 2 - Group 14.xlsx
+++ b/Assignment 2 - Group 14.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modro\Documents\GitHub\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EBC405-C45D-429A-BE8F-B9862772842B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AEA688-82EC-4A2E-A82D-CCE2E9099C26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Software Engineer - SDK (C++)</t>
   </si>
   <si>
-    <t>Moral Choice System Game - based around Batavia Mutiny of 1969</t>
-  </si>
-  <si>
     <t> Technical Lead @ Seventwenty </t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>links done, just need comments for reflecion</t>
+  </si>
+  <si>
+    <t>Moral Choice System Game - based around Batavia Mutiny of 1629</t>
   </si>
 </sst>
 </file>
@@ -919,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43:K44"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1023,7 +1023,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="34" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>73</v>
@@ -1061,10 +1061,10 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -1099,10 +1099,10 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1137,10 +1137,10 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1173,10 +1173,10 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1289,7 +1289,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>20</v>
@@ -1328,7 +1328,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
       <c r="K11" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1364,7 +1364,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
       <c r="K12" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1400,7 +1400,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="15"/>
       <c r="K13" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1461,7 +1461,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="2"/>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="16" spans="1:26" ht="26.25">
       <c r="A16" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="13" t="s">
@@ -1497,10 +1497,10 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K16" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -1533,7 +1533,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K17" s="40"/>
       <c r="L17" s="2"/>
@@ -1595,7 +1595,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
       <c r="J19" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="2"/>
@@ -1630,7 +1630,7 @@
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1723,7 +1723,7 @@
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
       <c r="J23" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K23" s="10"/>
       <c r="L23" s="2"/>
@@ -1855,7 +1855,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K27" s="10"/>
       <c r="L27" s="2"/>
@@ -1922,7 +1922,7 @@
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -1956,7 +1956,7 @@
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
       <c r="K30" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -1990,7 +1990,7 @@
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
       <c r="K31" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="32" spans="1:26" ht="15">
       <c r="A32" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
@@ -2024,7 +2024,7 @@
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -2085,7 +2085,7 @@
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
       <c r="J34" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K34" s="10"/>
       <c r="L34" s="2"/>
@@ -2114,17 +2114,17 @@
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K35" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -2160,7 +2160,7 @@
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -2186,7 +2186,7 @@
       <c r="C37" s="13"/>
       <c r="D37" s="15"/>
       <c r="E37" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -2194,7 +2194,7 @@
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
       <c r="K37" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
@@ -2750,7 +2750,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2780,7 +2780,7 @@
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2810,7 +2810,7 @@
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>

</xml_diff>

<commit_message>
final report doc drafted
Some comments to look at, plus a few gaps.
</commit_message>
<xml_diff>
--- a/Assignment 2 - Group 14.xlsx
+++ b/Assignment 2 - Group 14.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modro\Documents\GitHub\assignment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AEA688-82EC-4A2E-A82D-CCE2E9099C26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88791650-0512-42F9-80E1-1D6F300C2239}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -287,9 +287,6 @@
     <t>Machine Learning/AI</t>
   </si>
   <si>
-    <t>Nathan happy to work on layout for moment.  Something profesh :)</t>
-  </si>
-  <si>
     <t>Team Profile Website on Github</t>
   </si>
   <si>
@@ -320,17 +317,26 @@
     <t xml:space="preserve">Just via the submission page in canvas </t>
   </si>
   <si>
-    <t>links done, just need comments for reflecion</t>
+    <t>Moral Choice System Game - based around Batavia Mutiny of 1629</t>
   </si>
   <si>
-    <t>Moral Choice System Game - based around Batavia Mutiny of 1629</t>
+    <t>Website done with profile</t>
+  </si>
+  <si>
+    <t>Report drafted</t>
+  </si>
+  <si>
+    <t>Cory suggested adding the columns for currently held skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doesn't look like this is available yet.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -428,6 +434,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -514,7 +526,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -596,6 +608,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -919,8 +935,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1023,7 +1039,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K3" s="34" t="s">
         <v>73</v>
@@ -1289,7 +1305,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>20</v>
@@ -1461,9 +1477,11 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
-      <c r="K15" s="10"/>
+      <c r="K15" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1480,9 +1498,9 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="26.25">
+    <row r="16" spans="1:26" ht="25.5">
       <c r="A16" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="13" t="s">
@@ -1497,7 +1515,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="35" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="K16" s="38" t="s">
         <v>78</v>
@@ -1526,16 +1544,20 @@
       <c r="C17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="39" t="s">
+        <v>23</v>
+      </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
-      <c r="K17" s="40"/>
+      <c r="K17" s="38" t="s">
+        <v>78</v>
+      </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1595,7 +1617,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
       <c r="J19" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="2"/>
@@ -1614,7 +1636,7 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" spans="1:26" ht="15">
+    <row r="20" spans="1:26" ht="26.25">
       <c r="A20" s="11" t="s">
         <v>32</v>
       </c>
@@ -1626,9 +1648,13 @@
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="H20" s="40" t="s">
+        <v>23</v>
+      </c>
       <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
+      <c r="J20" s="41" t="s">
+        <v>97</v>
+      </c>
       <c r="K20" s="38" t="s">
         <v>78</v>
       </c>
@@ -1659,7 +1685,7 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="15" t="s">
+      <c r="I21" s="40" t="s">
         <v>23</v>
       </c>
       <c r="J21" s="15"/>
@@ -1723,9 +1749,11 @@
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
       <c r="J23" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
-      <c r="K23" s="10"/>
+      <c r="K23" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1855,9 +1883,11 @@
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
       <c r="J27" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
-      <c r="K27" s="10"/>
+      <c r="K27" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2085,9 +2115,11 @@
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
       <c r="J34" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
-      <c r="K34" s="10"/>
+      <c r="K34" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2114,14 +2146,14 @@
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K35" s="38" t="s">
         <v>78</v>
@@ -2152,7 +2184,7 @@
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -2186,7 +2218,7 @@
       <c r="C37" s="13"/>
       <c r="D37" s="15"/>
       <c r="E37" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -2280,25 +2312,27 @@
       <c r="C40" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G40" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="15" t="s">
+      <c r="I40" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="15"/>
+      <c r="J40" s="42" t="s">
+        <v>98</v>
+      </c>
       <c r="K40" s="40"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
@@ -2382,22 +2416,22 @@
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="15" t="s">
+      <c r="G43" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="H43" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="15" t="s">
+      <c r="I43" s="40" t="s">
         <v>23</v>
       </c>
       <c r="J43" s="28"/>
@@ -2426,12 +2460,24 @@
       <c r="C44" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
+      <c r="D44" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="H44" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" s="40" t="s">
+        <v>23</v>
+      </c>
       <c r="J44" s="28"/>
       <c r="K44" s="40"/>
       <c r="L44" s="2"/>
@@ -2750,7 +2796,7 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2780,7 +2826,7 @@
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2810,7 +2856,7 @@
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>

</xml_diff>

<commit_message>
Added reflection; updated assignment tracker doc.
</commit_message>
<xml_diff>
--- a/Assignment 2 - Group 14.xlsx
+++ b/Assignment 2 - Group 14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88791650-0512-42F9-80E1-1D6F300C2239}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262131F8-FFDA-4417-A361-DD79CEABC4EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -935,8 +935,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2416,11 +2416,11 @@
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
-      <c r="D43" s="40" t="s">
-        <v>23</v>
+      <c r="D43" s="37" t="s">
+        <v>89</v>
       </c>
-      <c r="E43" s="40" t="s">
-        <v>23</v>
+      <c r="E43" s="37" t="s">
+        <v>89</v>
       </c>
       <c r="F43" s="40" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
minor report edit only; updated assignment 2 tracking doc
</commit_message>
<xml_diff>
--- a/Assignment 2 - Group 14.xlsx
+++ b/Assignment 2 - Group 14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262131F8-FFDA-4417-A361-DD79CEABC4EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58FCA9B-3E66-435F-A90E-E39D9A2B1CE5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -329,7 +329,10 @@
     <t>Cory suggested adding the columns for currently held skills</t>
   </si>
   <si>
-    <t xml:space="preserve">doesn't look like this is available yet.  </t>
+    <t>Available from 11/04 - refer announcement</t>
+  </si>
+  <si>
+    <t>X update</t>
   </si>
 </sst>
 </file>
@@ -935,8 +938,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1649,7 +1652,7 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="40" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="I20" s="15"/>
       <c r="J20" s="41" t="s">
@@ -2312,10 +2315,10 @@
       <c r="C40" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="40" t="s">
+      <c r="D40" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="37" t="s">
         <v>23</v>
       </c>
       <c r="F40" s="40" t="s">

</xml_diff>

<commit_message>
Added industry data section to report
</commit_message>
<xml_diff>
--- a/Assignment 2 - Group 14.xlsx
+++ b/Assignment 2 - Group 14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58FCA9B-3E66-435F-A90E-E39D9A2B1CE5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7186DD39-5028-4CD1-9B40-3023A70EC7A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="100">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -332,7 +332,7 @@
     <t>Available from 11/04 - refer announcement</t>
   </si>
   <si>
-    <t>X update</t>
+    <t>X update (optional)</t>
   </si>
 </sst>
 </file>
@@ -938,8 +938,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1622,7 +1622,9 @@
       <c r="J19" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="K19" s="10"/>
+      <c r="K19" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1688,11 +1690,13 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
-      <c r="I21" s="40" t="s">
+      <c r="I21" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="38" t="s">
+        <v>78</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>

</xml_diff>

<commit_message>
added Cory, Nick and Harry's reflections to Report; updated assignment tracking doc
</commit_message>
<xml_diff>
--- a/Assignment 2 - Group 14.xlsx
+++ b/Assignment 2 - Group 14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7186DD39-5028-4CD1-9B40-3023A70EC7A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57748AB-6826-4F60-B7F4-E0F6A3A67E5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="102">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>X update (optional)</t>
+  </si>
+  <si>
+    <t>just Nathans to go</t>
+  </si>
+  <si>
+    <t>to do.</t>
   </si>
 </sst>
 </file>
@@ -938,8 +944,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2432,16 +2438,18 @@
       <c r="F43" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="40" t="s">
-        <v>23</v>
+      <c r="G43" s="37" t="s">
+        <v>89</v>
       </c>
-      <c r="H43" s="40" t="s">
-        <v>23</v>
+      <c r="H43" s="37" t="s">
+        <v>89</v>
       </c>
-      <c r="I43" s="40" t="s">
-        <v>23</v>
+      <c r="I43" s="37" t="s">
+        <v>89</v>
       </c>
-      <c r="J43" s="28"/>
+      <c r="J43" s="28" t="s">
+        <v>100</v>
+      </c>
       <c r="K43" s="40"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
@@ -2485,7 +2493,9 @@
       <c r="I44" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J44" s="28"/>
+      <c r="J44" s="28" t="s">
+        <v>101</v>
+      </c>
       <c r="K44" s="40"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>

</xml_diff>

<commit_message>
assignment tracking doc updated
</commit_message>
<xml_diff>
--- a/Assignment 2 - Group 14.xlsx
+++ b/Assignment 2 - Group 14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Documents\Lee\Intro to IT\Github\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57748AB-6826-4F60-B7F4-E0F6A3A67E5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C21951-CF75-4B29-95FA-D09BFE05389F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20052" yWindow="4092" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
   <si>
     <t>COSC2196 - Introduction to Information Technology</t>
   </si>
@@ -338,14 +338,14 @@
     <t>just Nathans to go</t>
   </si>
   <si>
-    <t>to do.</t>
+    <t>I was wrong ignore me.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -449,6 +449,41 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -535,7 +570,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,6 +656,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -944,8 +988,8 @@
   </sheetPr>
   <dimension ref="A1:Z1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1699,7 +1743,7 @@
       <c r="I21" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="40"/>
+      <c r="J21" s="2"/>
       <c r="K21" s="38" t="s">
         <v>78</v>
       </c>
@@ -2406,7 +2450,9 @@
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
       <c r="J42" s="9"/>
-      <c r="K42" s="10"/>
+      <c r="K42" s="47" t="s">
+        <v>20</v>
+      </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -2435,8 +2481,8 @@
       <c r="E43" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="F43" s="40" t="s">
-        <v>23</v>
+      <c r="F43" s="37" t="s">
+        <v>89</v>
       </c>
       <c r="G43" s="37" t="s">
         <v>89</v>
@@ -2450,7 +2496,7 @@
       <c r="J43" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="K43" s="40"/>
+      <c r="K43" s="16"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -2467,51 +2513,39 @@
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
     </row>
-    <row r="44" spans="1:26" ht="15">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:26" s="46" customFormat="1" ht="12.75">
+      <c r="A44" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11" t="s">
+      <c r="B44" s="43"/>
+      <c r="C44" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D44" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="G44" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="I44" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J44" s="28" t="s">
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="K44" s="40"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
-      <c r="X44" s="2"/>
-      <c r="Y44" s="2"/>
-      <c r="Z44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="45"/>
+      <c r="M44" s="45"/>
+      <c r="N44" s="45"/>
+      <c r="O44" s="45"/>
+      <c r="P44" s="45"/>
+      <c r="Q44" s="45"/>
+      <c r="R44" s="45"/>
+      <c r="S44" s="45"/>
+      <c r="T44" s="45"/>
+      <c r="U44" s="45"/>
+      <c r="V44" s="45"/>
+      <c r="W44" s="45"/>
+      <c r="X44" s="45"/>
+      <c r="Y44" s="45"/>
+      <c r="Z44" s="45"/>
     </row>
     <row r="45" spans="1:26" ht="12.75">
       <c r="A45" s="24"/>

</xml_diff>